<commit_message>
Subo pdf de Jira
</commit_message>
<xml_diff>
--- a/Testing/Casos_de_Prueba_Inventario.xlsx
+++ b/Testing/Casos_de_Prueba_Inventario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Users\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06C7C8D-D380-4D73-9AC5-DE4C51C043EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC58C9E5-EA5C-45F0-9101-E6B481593126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Alta de producto con datos correctos</t>
-  </si>
-  <si>
-    <t>Alta de producto sin nombre</t>
   </si>
   <si>
     <t>Acceso correcto al sistema</t>
@@ -172,23 +169,6 @@
   <si>
     <t xml:space="preserve">E-mail:
 Contraseña: </t>
-  </si>
-  <si>
-    <t>Nombre: Televisor ACECodigo: 0003
-Cantidad: 13
-Precio de costo: 80000
-Categoria existente: Tvs
-Agregar nueva categoria:
-Proveedor: Proovedor1</t>
-  </si>
-  <si>
-    <t>Nombre: 
-Codigo: 0004
-Cantidad: 12   
-Precio de costo: 70000
-Categoria existente: Heladeras
-Agregar nueva categoria:
-Proveedor: Proovedor1</t>
   </si>
   <si>
     <t>Nombre: Jorge
@@ -212,6 +192,37 @@
 Direccion:                                                  
 Telefono: 49540345                                                                                           
 E-mail: alex@alex.com </t>
+  </si>
+  <si>
+    <t>Nombre: Televisor ACE
+Codigo: 0003
+Cantidad: 13
+Precio de costo: 80000
+Categoria existente: Tvs
+Agregar nueva categoria:
+Proveedor: Proovedor1</t>
+  </si>
+  <si>
+    <t>Nombre: Heladera Net
+Codigo: 0004
+Cantidad: 12   
+Precio de costo: 70000
+Categoria existente: 
+Agregar nueva categoria:
+Proveedor: Proovedor1</t>
+  </si>
+  <si>
+    <t>Alta de producto sin Categoria</t>
+  </si>
+  <si>
+    <t>1. Acceder a gestion de proveedores.
+2. Presionar la opcion Agregar.
+3. Introducir los datos del Proveedor.
+4. Presionar en Agregar.
+5. Verificar el comportamiento del sistema.</t>
+  </si>
+  <si>
+    <t>TC-009</t>
   </si>
 </sst>
 </file>
@@ -597,38 +608,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="3" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7265625" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
     <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" customWidth="1"/>
-    <col min="8" max="8" width="19.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -637,36 +648,36 @@
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2">
         <v>45853</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -674,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2">
         <v>45853</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -700,25 +711,25 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="2">
         <v>45853</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -726,126 +737,152 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="2">
         <v>45853</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="99.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="2">
         <v>45853</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="2">
         <v>45853</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="2">
         <v>45853</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="2">
         <v>45853</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="2">
+        <v>45854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>